<commit_message>
made export, clear button, revise design
</commit_message>
<xml_diff>
--- a/export.xlsx
+++ b/export.xlsx
@@ -345,7 +345,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A31"/>
+  <dimension ref="A1:B31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -363,7 +363,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2020-03-06 16:08:30.248187</t>
+          <t>2020-03-12 20:30:54.168122</t>
         </is>
       </c>
     </row>
@@ -377,6 +377,11 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
+          <t xml:space="preserve">Fwd mean draft, m: </t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
           <t>2.0</t>
         </is>
       </c>
@@ -384,6 +389,11 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
+          <t xml:space="preserve">Middle mean draft, m: </t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
           <t>2.0</t>
         </is>
       </c>
@@ -391,6 +401,11 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
+          <t xml:space="preserve">Aft mean draft, m: </t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
           <t>2.0</t>
         </is>
       </c>
@@ -398,6 +413,11 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
+          <t xml:space="preserve">Fwd mark misplacement, m: </t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
           <t>-2.095</t>
         </is>
       </c>
@@ -405,6 +425,11 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
+          <t xml:space="preserve">Mid mark misplacement, m: </t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
           <t>1.078</t>
         </is>
       </c>
@@ -412,6 +437,11 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
+          <t xml:space="preserve">Aft mark misplacement, m: </t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
           <t>3.067</t>
         </is>
       </c>
@@ -419,6 +449,11 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
+          <t xml:space="preserve">Apparent trim, m: </t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
           <t>0.0</t>
         </is>
       </c>
@@ -426,6 +461,11 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
+          <t xml:space="preserve">Fwd draft correction, m: </t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
           <t>-0.0</t>
         </is>
       </c>
@@ -433,6 +473,11 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
+          <t xml:space="preserve">Mid draft correction, m: </t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
           <t>0.0</t>
         </is>
       </c>
@@ -440,6 +485,11 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
+          <t xml:space="preserve">Aft draft correction, m: </t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
           <t>0.0</t>
         </is>
       </c>
@@ -447,6 +497,11 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
+          <t xml:space="preserve">Fwd corrected draft, m: </t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
           <t>2.0</t>
         </is>
       </c>
@@ -454,6 +509,11 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
+          <t xml:space="preserve">Mid corrected draft, m: </t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
           <t>2.0</t>
         </is>
       </c>
@@ -461,6 +521,11 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
+          <t xml:space="preserve">Aft corrected draft, m: </t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
           <t>2.0</t>
         </is>
       </c>
@@ -468,6 +533,11 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
+          <t xml:space="preserve">True trim, m: </t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
           <t>0.0</t>
         </is>
       </c>
@@ -475,6 +545,11 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
+          <t xml:space="preserve">Deflection: </t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
           <t>Hogging - Выгиб</t>
         </is>
       </c>
@@ -482,6 +557,11 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
+          <t>Mean of means corrected, m:</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
           <t>2.0</t>
         </is>
       </c>
@@ -489,6 +569,11 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
+          <t xml:space="preserve">Displacement by MOMC, mt: </t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
           <t>2926.49</t>
         </is>
       </c>
@@ -496,6 +581,11 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
+          <t xml:space="preserve">TPC, mt: </t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
           <t>16.05</t>
         </is>
       </c>
@@ -503,6 +593,11 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
+          <t xml:space="preserve">LCF, m: </t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
           <t>64.796</t>
         </is>
       </c>
@@ -510,6 +605,11 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
+          <t>First trim correction, mt:</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
           <t>0.0</t>
         </is>
       </c>
@@ -517,6 +617,11 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
+          <t xml:space="preserve">MTC by MOMC: </t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
           <t>106.77</t>
         </is>
       </c>
@@ -524,6 +629,11 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
+          <t xml:space="preserve">MTC +: </t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
           <t>110.69</t>
         </is>
       </c>
@@ -531,6 +641,11 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
+          <t xml:space="preserve">MTC -: </t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
           <t>101.77</t>
         </is>
       </c>
@@ -538,6 +653,11 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
+          <t xml:space="preserve">MTC difference: </t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
           <t>8.92</t>
         </is>
       </c>
@@ -545,6 +665,11 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
+          <t>Second trim correction, mt:</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
           <t>0.0</t>
         </is>
       </c>
@@ -552,6 +677,11 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
+          <t xml:space="preserve">Disp. corrected by trim, mt: </t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
           <t>2926.49</t>
         </is>
       </c>
@@ -559,12 +689,22 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
+          <t xml:space="preserve">Constant, mt: </t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
           <t>-1142.877</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Displacement corrected, mt: </t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
         <is>
           <t>2926.49</t>
         </is>

</xml_diff>